<commit_message>
Removing unused connections from the file
</commit_message>
<xml_diff>
--- a/SSASDatabasesDataComparison.xlsx
+++ b/SSASDatabasesDataComparison.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="0" windowWidth="19080" windowHeight="7380"/>
+    <workbookView xWindow="2820" yWindow="0" windowWidth="19080" windowHeight="7380"/>
   </bookViews>
   <sheets>
-    <sheet name="All measures without errors" sheetId="5" r:id="rId1"/>
+    <sheet name="differences discovery start scr" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="585" r:id="rId2"/>
+    <pivotCache cacheId="7" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,19 +28,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\serge_000\Documents\Мои источники данных\. AdventureWorksDW2014Multidimensional-EE Adventure Works.odc" keepAlive="1" name=". AdventureWorksDW2014Multidimensional-EE Adventure Works" type="5" refreshedVersion="5" background="1">
-    <dbPr connection="Provider=MSOLAP.6;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=AdventureWorksDW2014Multidimensional-EE;Data Source=.;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error" command="Adventure Works" commandType="1"/>
-    <olapPr sendLocale="1" rowDrillCount="1000"/>
-  </connection>
-  <connection id="2" odcFile="C:\Users\serge_000\Documents\Мои источники данных\. AdventureWorksDW2014Multidimensional-EE Adventure Works.odc" keepAlive="1" name=". AdventureWorksDW2014Multidimensional-EE Adventure Works1" type="5" refreshedVersion="5" background="1">
-    <dbPr connection="Provider=MSOLAP.6;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=AdventureWorksDW2014Multidimensional-EE;Data Source=.;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error" command="Adventure Works" commandType="1"/>
-    <olapPr sendLocale="1" rowDrillCount="1000"/>
-  </connection>
-  <connection id="3" odcFile="C:\Users\serge_000\Documents\Мои источники данных\. AdventureWorksDW2014Multidimensional-EE Adventure Works.odc" keepAlive="1" name=". AdventureWorksDW2014Multidimensional-EE Adventure Works2" type="5" refreshedVersion="5" background="1">
-    <dbPr connection="Provider=MSOLAP.6;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=AdventureWorksDW2014Multidimensional-EE;Data Source=.;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error" command="Adventure Works" commandType="1"/>
-    <olapPr sendLocale="1" rowDrillCount="1000"/>
-  </connection>
-  <connection id="4" odcFile="C:\Users\serge_000\Documents\Мои источники данных\. AdventureWorksDW2014Multidimensional-EE Adventure Works.odc" keepAlive="1" name=". AdventureWorksDW2014Multidimensional-EE Adventure Works3" type="5" refreshedVersion="5" background="1">
+  <connection id="1" odcFile="C:\Users\serge_000\Documents\Мои источники данных\. AdventureWorksDW2014Multidimensional-EE Adventure Works.odc" keepAlive="1" name=". AdventureWorksDW2014Multidimensional-EE Adventure Works3" type="5" refreshedVersion="5" background="1" saveData="1">
     <dbPr connection="Provider=MSOLAP.6;Integrated Security=SSPI;Persist Security Info=True;Initial Catalog=AdventureWorksDW2014Multidimensional-EE;Data Source=.;MDX Compatibility=1;Safety Options=2;MDX Missing Member Mode=Error" command="Adventure Works" commandType="1"/>
     <olapPr sendLocale="1" rowDrillCount="1000"/>
   </connection>
@@ -195,7 +183,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,###"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00_);\([$$-409]#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="#,###.00"/>
+    <numFmt numFmtId="166" formatCode="#,###.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -234,7 +222,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -254,8 +242,8 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="sergey.a.vdovin@gmail.com" refreshedDate="42309.712529861114" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
-  <cacheSource type="external" connectionId="4"/>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="sergey.a.vdovin@gmail.com" refreshedDate="42309.737504861114" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="1"/>
   <cacheFields count="42">
     <cacheField name="[Comparison Operations].[Comparison Operations].[Comparison Operations]" caption="Comparison Operations" numFmtId="0" hierarchy="3" level="1">
       <sharedItems count="3">
@@ -947,7 +935,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="СводнаяТаблица6" cacheId="585" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="СводнаяТаблица6" cacheId="7" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:D43" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="42">
     <pivotField axis="axisCol" allDrilled="1" showAll="0" defaultAttributeDrillState="1">
@@ -1160,9 +1148,11 @@
     <dataField fld="15" baseField="0" baseItem="0"/>
     <dataField fld="16" baseField="0" baseItem="0"/>
     <dataField fld="17" baseField="0" baseItem="0"/>
+    <dataField fld="35" baseField="0" baseItem="0"/>
     <dataField fld="18" baseField="0" baseItem="0"/>
     <dataField fld="19" baseField="0" baseItem="0"/>
     <dataField fld="20" baseField="0" baseItem="0"/>
+    <dataField fld="37" baseField="0" baseItem="0"/>
     <dataField fld="21" baseField="0" baseItem="0"/>
     <dataField fld="22" baseField="0" baseItem="0"/>
     <dataField fld="23" baseField="0" baseItem="0"/>
@@ -1177,9 +1167,7 @@
     <dataField fld="32" baseField="0" baseItem="0"/>
     <dataField fld="33" baseField="0" baseItem="0"/>
     <dataField fld="34" baseField="0" baseItem="0"/>
-    <dataField fld="35" baseField="0" baseItem="0"/>
     <dataField fld="36" baseField="0" baseItem="0"/>
-    <dataField fld="37" baseField="0" baseItem="0"/>
     <dataField fld="38" baseField="0" baseItem="0"/>
     <dataField fld="39" baseField="0" baseItem="0"/>
     <dataField fld="40" baseField="0" baseItem="0"/>
@@ -1800,16 +1788,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -2087,247 +2075,247 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6">
-        <v>6.556917487089118E-3</v>
-      </c>
-      <c r="C20" s="6">
-        <v>6.556917487089118E-3</v>
-      </c>
-      <c r="D20" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="B20" s="4">
+        <v>12551367.248302758</v>
+      </c>
+      <c r="C20" s="4">
+        <v>12551366.248302758</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4">
-        <v>21193.518699236036</v>
-      </c>
-      <c r="C21" s="4">
-        <v>21193.518699236036</v>
-      </c>
-      <c r="D21" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="6">
+        <v>6.556917487089118E-3</v>
+      </c>
+      <c r="C21" s="6">
+        <v>6.556917487089118E-3</v>
+      </c>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>444.4311190633473</v>
+        <v>21193.518699236036</v>
       </c>
       <c r="C22" s="4">
-        <v>444.4311190633473</v>
+        <v>21193.518699236036</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="4">
-        <v>80978104.870700002</v>
+        <v>444.4311190633473</v>
       </c>
       <c r="C23" s="4">
-        <v>80978104.870700002</v>
+        <v>444.4311190633473</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4">
-        <v>2011265.9158000001</v>
+        <v>109809275.2030015</v>
       </c>
       <c r="C24" s="4">
-        <v>2011265.9158000001</v>
-      </c>
-      <c r="D24" s="4"/>
+        <v>109809274.2030015</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="4">
-        <v>470482.60330000002</v>
+        <v>80978104.870700002</v>
       </c>
       <c r="C25" s="4">
-        <v>470482.60330000002</v>
+        <v>80978104.870700002</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="6">
-        <v>5.8480933759075928E-3</v>
-      </c>
-      <c r="C26" s="6">
-        <v>5.8480933759075928E-3</v>
-      </c>
-      <c r="D26" s="6"/>
+        <v>23</v>
+      </c>
+      <c r="B26" s="4">
+        <v>2011265.9158000001</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2011265.9158000001</v>
+      </c>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="3">
-        <v>214378</v>
-      </c>
-      <c r="C27" s="3">
-        <v>214378</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B27" s="4">
+        <v>470482.60330000002</v>
+      </c>
+      <c r="C27" s="4">
+        <v>470482.60330000002</v>
+      </c>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B28" s="6">
-        <v>1</v>
+        <v>5.8480933759075928E-3</v>
       </c>
       <c r="C28" s="6">
-        <v>1</v>
+        <v>5.8480933759075928E-3</v>
       </c>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="4">
-        <v>80450596.982299998</v>
-      </c>
-      <c r="C29" s="4">
-        <v>80450596.982299998</v>
-      </c>
-      <c r="D29" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="B29" s="3">
+        <v>214378</v>
+      </c>
+      <c r="C29" s="3">
+        <v>214378</v>
+      </c>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="4">
-        <v>26693830.572700001</v>
-      </c>
-      <c r="C30" s="4">
-        <v>26693830.572700001</v>
-      </c>
-      <c r="D30" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B31" s="4">
-        <v>6436047.6065999996</v>
+        <v>80450596.982299998</v>
       </c>
       <c r="C31" s="4">
-        <v>6436047.6065999996</v>
+        <v>80450596.982299998</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="4">
-        <v>79980114.378999993</v>
+        <v>26693830.572700001</v>
       </c>
       <c r="C32" s="4">
-        <v>79980114.378999993</v>
+        <v>26693830.572700001</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B33" s="4">
-        <v>465.18051488458735</v>
+        <v>6436047.6065999996</v>
       </c>
       <c r="C33" s="4">
-        <v>465.18051488458735</v>
+        <v>6436047.6065999996</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="6">
-        <v>0.25190830600477271</v>
-      </c>
-      <c r="C34" s="6">
-        <v>0.25190830829882582</v>
-      </c>
-      <c r="D34" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="B34" s="4">
+        <v>79980114.378999993</v>
+      </c>
+      <c r="C34" s="4">
+        <v>79980114.378999993</v>
+      </c>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B35" s="4">
-        <v>110336782.09140149</v>
+        <v>465.18051488458735</v>
       </c>
       <c r="C35" s="4">
-        <v>110336782.09140149</v>
+        <v>465.18051488458735</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="4">
-        <v>2745235.5248999768</v>
-      </c>
-      <c r="C36" s="4">
-        <v>2745235.5248999768</v>
-      </c>
-      <c r="D36" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0.25190830600477271</v>
+      </c>
+      <c r="C36" s="6">
+        <v>0.25190830829882582</v>
+      </c>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B37" s="4">
-        <v>12551367.248302758</v>
+        <v>110336782.09140149</v>
       </c>
       <c r="C37" s="4">
-        <v>12551366.248302758</v>
-      </c>
-      <c r="D37" s="4">
-        <v>1</v>
-      </c>
+        <v>110336782.09140149</v>
+      </c>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="3">
-        <v>274776</v>
-      </c>
-      <c r="C38" s="3">
-        <v>274776</v>
-      </c>
-      <c r="D38" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="B38" s="4">
+        <v>2745235.5248999768</v>
+      </c>
+      <c r="C38" s="4">
+        <v>2745235.5248999768</v>
+      </c>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="4">
-        <v>109809275.2030015</v>
-      </c>
-      <c r="C39" s="4">
-        <v>109809274.2030015</v>
-      </c>
-      <c r="D39" s="4">
-        <v>1</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B39" s="3">
+        <v>274776</v>
+      </c>
+      <c r="C39" s="3">
+        <v>274776</v>
+      </c>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">

</xml_diff>